<commit_message>
Bomben legen - stehen noch
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -1984,13 +1984,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0</c:v>
@@ -2002,7 +2002,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0</c:v>
@@ -2230,7 +2230,7 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2746,7 +2746,7 @@
   <dimension ref="A1:AX42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="AB26" sqref="AB26"/>
+      <selection activeCell="AJ20" sqref="AJ20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3570,7 +3570,7 @@
       </c>
       <c r="D14" s="44">
         <f>SUM(D15:D21)</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E14" s="45"/>
       <c r="F14" s="50"/>
@@ -3624,7 +3624,7 @@
       </c>
       <c r="D15" s="88">
         <f>SUM(I15:AQ15)</f>
-        <v>15.5</v>
+        <v>25.5</v>
       </c>
       <c r="E15" s="85">
         <v>1</v>
@@ -3659,14 +3659,20 @@
       <c r="AA15" s="73"/>
       <c r="AB15" s="90"/>
       <c r="AC15" s="92"/>
-      <c r="AD15" s="73"/>
+      <c r="AD15" s="73">
+        <v>2</v>
+      </c>
       <c r="AE15" s="71"/>
-      <c r="AF15" s="71"/>
+      <c r="AF15" s="71">
+        <v>1</v>
+      </c>
       <c r="AG15" s="90"/>
       <c r="AH15" s="97"/>
       <c r="AI15" s="98"/>
-      <c r="AJ15" s="20"/>
-      <c r="AK15" s="20"/>
+      <c r="AJ15" s="73">
+        <v>7</v>
+      </c>
+      <c r="AK15" s="73"/>
       <c r="AL15" s="105"/>
       <c r="AM15" s="97"/>
       <c r="AN15" s="98"/>
@@ -5133,7 +5139,7 @@
       </c>
       <c r="D42" s="57">
         <f>SUM(D39+D37+D33+D14+D10+D5)</f>
-        <v>50.5</v>
+        <v>60.5</v>
       </c>
       <c r="E42" s="57"/>
       <c r="F42" s="57"/>
@@ -5225,7 +5231,7 @@
       </c>
       <c r="AD42" s="57">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE42" s="61">
         <f t="shared" si="4"/>
@@ -5233,7 +5239,7 @@
       </c>
       <c r="AF42" s="57">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG42" s="61">
         <f t="shared" si="4"/>
@@ -5249,7 +5255,7 @@
       </c>
       <c r="AJ42" s="61">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK42" s="57">
         <f t="shared" si="4"/>
@@ -5579,7 +5585,7 @@
       </c>
       <c r="B25" s="66">
         <f>Zeitplanung!AD42</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5599,7 +5605,7 @@
       </c>
       <c r="B27" s="66">
         <f>Zeitplanung!AF42</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5639,7 +5645,7 @@
       </c>
       <c r="B31" s="66">
         <f>Zeitplanung!AJ42</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5715,7 +5721,7 @@
       </c>
       <c r="D39" s="66">
         <f>Zeitplanung!D14</f>
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>